<commit_message>
arc() function documentation cite
</commit_message>
<xml_diff>
--- a/data/image1.xlsx
+++ b/data/image1.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="image1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -366,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -407,198 +407,224 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1.6793981481481483E-2</v>
+      <c r="A2">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>731</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.125149803</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <f>F2*360</f>
-        <v>45.053929080000003</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <f>G2</f>
-        <v>45.053929080000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>5.8634259259259254E-2</v>
+        <v>1.6793981481481483E-2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>24</v>
       </c>
       <c r="D3">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E3">
-        <v>2546</v>
+        <v>731</v>
       </c>
       <c r="F3">
-        <v>0.43588426600000002</v>
+        <v>0.125149803</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G8" si="0">F3*360</f>
-        <v>156.91833576000002</v>
+        <f>F3*360</f>
+        <v>45.053929080000003</v>
       </c>
       <c r="H3">
-        <f>G3-G2</f>
-        <v>111.86440668000002</v>
+        <f>G3</f>
+        <v>45.053929080000003</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>7.4467592592592599E-2</v>
+        <v>5.8634259259259254E-2</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
+        <v>24</v>
+      </c>
+      <c r="D4">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>2546</v>
+      </c>
+      <c r="F4">
+        <v>0.43588426600000002</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G9" si="0">F4*360</f>
+        <v>156.91833576000002</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H9" si="1">G4-G3</f>
+        <v>111.86440668000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>7.4467592592592599E-2</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>47</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>14</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>3224</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>0.55196028100000005</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>198.70570116000002</v>
       </c>
-      <c r="H4">
-        <f>G4-G3</f>
+      <c r="H5">
+        <f t="shared" si="1"/>
         <v>41.787365399999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>0.10347222222222223</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>29</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>4470</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>0.76527991799999995</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>275.50077047999997</v>
       </c>
-      <c r="H5">
-        <f>G5-G4</f>
+      <c r="H6">
+        <f t="shared" si="1"/>
         <v>76.795069319999953</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>0.11464120370370372</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>45</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>4955</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>0.84831364499999995</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <f t="shared" si="0"/>
         <v>305.39291219999996</v>
       </c>
-      <c r="H6">
-        <f>G6-G5</f>
+      <c r="H7">
+        <f t="shared" si="1"/>
         <v>29.892141719999984</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>0.12716435185185185</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>3</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>7</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>5497</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>0.94110597500000004</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <f t="shared" si="0"/>
         <v>338.79815100000002</v>
       </c>
-      <c r="H7">
-        <f>G7-G6</f>
+      <c r="H8">
+        <f t="shared" si="1"/>
         <v>33.405238800000063</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>0.13496527777777778</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>14</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>21</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>5841</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>1</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <f t="shared" si="0"/>
         <v>360</v>
       </c>
-      <c r="H8">
-        <f>G8-G7</f>
+      <c r="H9">
+        <f t="shared" si="1"/>
         <v>21.201848999999982</v>
       </c>
     </row>

</xml_diff>